<commit_message>
BASIC lighting functions no CAN
</commit_message>
<xml_diff>
--- a/hardware/pinAssignments.xlsx
+++ b/hardware/pinAssignments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pacific Lab\git\electrekTaillight\trekTaillight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pacific Lab\Documents\Projects\STM32\trekTaillight\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B02610F-899B-4243-B356-7E23DDB6B502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D3163C-A76B-48C5-95FA-B01C74FF909F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1877B3B1-3179-4C18-8060-FC16BC521077}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{1877B3B1-3179-4C18-8060-FC16BC521077}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>TailLight Pin Assignments</t>
   </si>
@@ -71,12 +71,6 @@
     <t>PB1</t>
   </si>
   <si>
-    <t>Brake light enable pin.</t>
-  </si>
-  <si>
-    <t>Backup light enable pin.</t>
-  </si>
-  <si>
     <t>RED_EN</t>
   </si>
   <si>
@@ -122,9 +116,6 @@
     <t>PA6</t>
   </si>
   <si>
-    <t>External load switch enable (used for powering ON/OFF turn signal)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Select R27 for VLED 48V (default) or Select R28 for 12V mode. </t>
   </si>
   <si>
@@ -198,6 +189,24 @@
   </si>
   <si>
     <t>Enabled by default</t>
+  </si>
+  <si>
+    <t>AF_PWM</t>
+  </si>
+  <si>
+    <t>PWM push pull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWM push pull </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brake light enable pin. TIM3 Ch3 </t>
+  </si>
+  <si>
+    <t>Backup light enable pin. TIM3 Ch4</t>
+  </si>
+  <si>
+    <t>EXT Switch TIM3 Ch1  (TURN EN)</t>
   </si>
 </sst>
 </file>
@@ -259,9 +268,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -299,7 +308,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -405,7 +414,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -547,7 +556,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -558,7 +567,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -599,10 +608,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -613,172 +625,175 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
         <v>49</v>
-      </c>
-      <c r="D16" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>